<commit_message>
More work on calibration paper, mostly related work, but also added translation only calibration tests.
</commit_message>
<xml_diff>
--- a/calibration/overall_stats_cal_9_15_premo_cmu.xlsx
+++ b/calibration/overall_stats_cal_9_15_premo_cmu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_papers\calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_cal_data\cal_9_15_premo_cmu\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B421ABC-BD86-4B34-99F7-FED6084A8717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C0CA2-4FBD-4D53-8055-83CC9FAB227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="8748" windowWidth="15060" windowHeight="8508" activeTab="2" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="34560" windowHeight="19140" activeTab="2" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Error stats" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>Calibration</t>
   </si>
@@ -83,6 +83,9 @@
     <t>XYZ_all_concentric_hr_cal</t>
   </si>
   <si>
+    <t>trans_only_hr_cal</t>
+  </si>
+  <si>
     <t>default</t>
   </si>
   <si>
@@ -95,7 +98,7 @@
     <t>sf nocorrect</t>
   </si>
   <si>
-    <t>sfnp noZout</t>
+    <t>trans only noc</t>
   </si>
   <si>
     <t>output/XYZ_nosofix_hr_cal</t>
@@ -114,6 +117,9 @@
   </si>
   <si>
     <t>output\XYZ_all_hr_cal</t>
+  </si>
+  <si>
+    <t>output/trans_only_hr_cal</t>
   </si>
 </sst>
 </file>
@@ -234,10 +240,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -580,35 +586,35 @@
         <v>5</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
       <c r="J1" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S1" s="17"/>
       <c r="T1" s="17"/>
-      <c r="U1" s="19"/>
+      <c r="U1" s="18"/>
       <c r="V1" s="16"/>
       <c r="W1" s="17"/>
       <c r="X1" s="17"/>
@@ -616,65 +622,65 @@
       <c r="Z1" s="16"/>
       <c r="AA1" s="17"/>
       <c r="AB1" s="17"/>
-      <c r="AC1" s="19"/>
+      <c r="AC1" s="18"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="17"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="K2" s="17"/>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="19"/>
       <c r="N2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="O2" s="17"/>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="18"/>
+      <c r="Q2" s="19"/>
       <c r="R2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="S2" s="17"/>
-      <c r="T2" s="18" t="s">
+      <c r="T2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="18"/>
+      <c r="U2" s="19"/>
       <c r="V2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="W2" s="17"/>
-      <c r="X2" s="18" t="s">
+      <c r="X2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="18"/>
+      <c r="Y2" s="19"/>
       <c r="Z2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="AA2" s="17"/>
-      <c r="AB2" s="18" t="s">
+      <c r="AB2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="18"/>
+      <c r="AC2" s="19"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -770,10 +776,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="7">
-        <v>0.28344638376068243</v>
+        <v>0.28068832614114686</v>
       </c>
       <c r="C4" s="8">
-        <v>0.76680325619476697</v>
+        <v>0.73440433276177086</v>
       </c>
       <c r="D4" s="8">
         <v>0.27469341877840853</v>
@@ -782,10 +788,10 @@
         <v>0.64227560401111072</v>
       </c>
       <c r="F4" s="7">
-        <v>0.45156805827987784</v>
+        <v>0.4334366747998819</v>
       </c>
       <c r="G4" s="8">
-        <v>1.3044023148183825</v>
+        <v>1.0968607376832644</v>
       </c>
       <c r="H4" s="8">
         <v>0.27469341877840853</v>
@@ -794,10 +800,10 @@
         <v>0.64227560401111072</v>
       </c>
       <c r="J4" s="7">
-        <v>5.7184619429376182</v>
+        <v>5.7193779810343397</v>
       </c>
       <c r="K4" s="8">
-        <v>12.707946315292794</v>
+        <v>12.664857302939918</v>
       </c>
       <c r="L4" s="8">
         <v>1.8246372218996534</v>
@@ -806,10 +812,10 @@
         <v>5.2159749292658475</v>
       </c>
       <c r="N4" s="7">
-        <v>4.5594831352365901</v>
+        <v>4.5757703431194194</v>
       </c>
       <c r="O4" s="8">
-        <v>12.344549508447102</v>
+        <v>12.402570780535587</v>
       </c>
       <c r="P4" s="8">
         <v>1.8246372218996534</v>
@@ -818,16 +824,16 @@
         <v>5.2159749292658475</v>
       </c>
       <c r="R4" s="7">
-        <v>4.6664987851134594</v>
+        <v>0.44045419156778232</v>
       </c>
       <c r="S4" s="8">
-        <v>12.34451775671857</v>
+        <v>1.0620358317544398</v>
       </c>
       <c r="T4" s="8">
-        <v>1.8205815184244147</v>
+        <v>0.26942241141433476</v>
       </c>
       <c r="U4" s="8">
-        <v>5.2159253295478525</v>
+        <v>0.48903093956696497</v>
       </c>
       <c r="V4" s="7"/>
       <c r="W4" s="8"/>
@@ -843,10 +849,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="7">
-        <v>0.87793323047682681</v>
+        <v>0.89609555096667726</v>
       </c>
       <c r="C5" s="8">
-        <v>2.0962676481595031</v>
+        <v>2.1941738410909193</v>
       </c>
       <c r="D5" s="8">
         <v>0.53910231829652577</v>
@@ -855,10 +861,10 @@
         <v>1.3845684193091312</v>
       </c>
       <c r="F5" s="7">
-        <v>0.87793323047682681</v>
+        <v>0.89609555096667726</v>
       </c>
       <c r="G5" s="8">
-        <v>2.0962676481595031</v>
+        <v>2.1941738410909193</v>
       </c>
       <c r="H5" s="8">
         <v>0.53910231829652577</v>
@@ -867,10 +873,10 @@
         <v>1.3845684193091312</v>
       </c>
       <c r="J5" s="7">
-        <v>2.2710956871302348</v>
+        <v>2.2963169785338899</v>
       </c>
       <c r="K5" s="8">
-        <v>5.9312366381643784</v>
+        <v>5.9709407594525068</v>
       </c>
       <c r="L5" s="8">
         <v>1.0974303795083338</v>
@@ -879,10 +885,10 @@
         <v>3.400564659715593</v>
       </c>
       <c r="N5" s="7">
-        <v>2.2710956871302348</v>
+        <v>2.2963169785338899</v>
       </c>
       <c r="O5" s="8">
-        <v>5.9312366381643784</v>
+        <v>5.9709407594525068</v>
       </c>
       <c r="P5" s="8">
         <v>1.0974303795083338</v>
@@ -891,16 +897,16 @@
         <v>3.400564659715593</v>
       </c>
       <c r="R5" s="7">
-        <v>2.2886656314373122</v>
+        <v>0.86048770947841613</v>
       </c>
       <c r="S5" s="8">
-        <v>5.931237893093031</v>
+        <v>1.746219106615871</v>
       </c>
       <c r="T5" s="8">
-        <v>1.1078472048848054</v>
+        <v>0.4013744777622526</v>
       </c>
       <c r="U5" s="8">
-        <v>3.400565742558662</v>
+        <v>0.89751579883269172</v>
       </c>
       <c r="V5" s="7"/>
       <c r="W5" s="8"/>
@@ -916,10 +922,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="7">
-        <v>0.47004109666478622</v>
+        <v>0.47338873693850109</v>
       </c>
       <c r="C6" s="8">
-        <v>1.2679053176800132</v>
+        <v>1.2639406414266798</v>
       </c>
       <c r="D6" s="8">
         <v>0.51090298228368991</v>
@@ -928,10 +934,10 @@
         <v>1.4147130140210986</v>
       </c>
       <c r="F6" s="7">
-        <v>0.87729002129534805</v>
+        <v>0.89970080651660578</v>
       </c>
       <c r="G6" s="8">
-        <v>2.5765351802957399</v>
+        <v>2.5883718045785824</v>
       </c>
       <c r="H6" s="8">
         <v>0.51090298228368991</v>
@@ -940,10 +946,10 @@
         <v>1.4147130140210986</v>
       </c>
       <c r="J6" s="7">
-        <v>17.57360883404079</v>
+        <v>17.567171757536862</v>
       </c>
       <c r="K6" s="8">
-        <v>34.092939588124864</v>
+        <v>34.079012611828539</v>
       </c>
       <c r="L6" s="8">
         <v>1.7777301511231276</v>
@@ -952,10 +958,10 @@
         <v>6.0029184201631915</v>
       </c>
       <c r="N6" s="7">
-        <v>4.3664245762997043</v>
+        <v>4.389302757355825</v>
       </c>
       <c r="O6" s="8">
-        <v>13.018497547393</v>
+        <v>13.090889322656274</v>
       </c>
       <c r="P6" s="8">
         <v>1.7777301511231276</v>
@@ -964,16 +970,16 @@
         <v>6.0029184201631915</v>
       </c>
       <c r="R6" s="7">
-        <v>3.8675890659838115</v>
+        <v>0.77313860393405931</v>
       </c>
       <c r="S6" s="8">
-        <v>13.018497547393</v>
+        <v>1.911153534215704</v>
       </c>
       <c r="T6" s="8">
-        <v>1.5417404897786977</v>
+        <v>0.44334559757633096</v>
       </c>
       <c r="U6" s="8">
-        <v>6.0029184201631915</v>
+        <v>0.94597671130165861</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" s="8"/>
@@ -989,10 +995,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="7">
-        <v>2.0615782659916975</v>
+        <v>2.0960226951338661</v>
       </c>
       <c r="C7" s="8">
-        <v>4.8397161368991757</v>
+        <v>4.8527739510808656</v>
       </c>
       <c r="D7" s="8">
         <v>1.1048633974423512</v>
@@ -1001,10 +1007,10 @@
         <v>2.857977074784988</v>
       </c>
       <c r="F7" s="7">
-        <v>2.0615782659916975</v>
+        <v>2.0960226951338661</v>
       </c>
       <c r="G7" s="8">
-        <v>4.8397161368991757</v>
+        <v>4.8527739510808656</v>
       </c>
       <c r="H7" s="8">
         <v>1.1048633974423512</v>
@@ -1013,10 +1019,10 @@
         <v>2.857977074784988</v>
       </c>
       <c r="J7" s="7">
-        <v>3.3245549638751219</v>
+        <v>3.3593786984465095</v>
       </c>
       <c r="K7" s="8">
-        <v>9.1359952207083257</v>
+        <v>9.1628312648326293</v>
       </c>
       <c r="L7" s="8">
         <v>1.6483812491916423</v>
@@ -1025,10 +1031,10 @@
         <v>4.9694351523684492</v>
       </c>
       <c r="N7" s="7">
-        <v>3.3245549638751219</v>
+        <v>3.3593786984465095</v>
       </c>
       <c r="O7" s="8">
-        <v>9.1359952207083257</v>
+        <v>9.1628312648326293</v>
       </c>
       <c r="P7" s="8">
         <v>1.6483812491916423</v>
@@ -1037,16 +1043,16 @@
         <v>4.9694351523684492</v>
       </c>
       <c r="R7" s="7">
-        <v>2.8021695149375483</v>
+        <v>1.8533410856640939</v>
       </c>
       <c r="S7" s="8">
-        <v>8.1239492874040202</v>
+        <v>3.8765000070625075</v>
       </c>
       <c r="T7" s="8">
-        <v>1.4166433989658647</v>
+        <v>0.969492110720096</v>
       </c>
       <c r="U7" s="8">
-        <v>4.5981470991266047</v>
+        <v>2.0090363659847279</v>
       </c>
       <c r="V7" s="7"/>
       <c r="W7" s="8"/>
@@ -1058,26 +1064,69 @@
       <c r="AC7" s="8"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2.0161262455969489</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6.0723151510827398</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1.1608734504931362</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.0251112642908211</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2.0195603550988559</v>
+      </c>
+      <c r="G8" s="8">
+        <v>6.2161674725761831</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.1608734504931362</v>
+      </c>
+      <c r="I8" s="8">
+        <v>3.0251112642908211</v>
+      </c>
+      <c r="J8" s="7">
+        <v>4.0425154984316869</v>
+      </c>
+      <c r="K8" s="8">
+        <v>10.319847881624611</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1.8197530409203637</v>
+      </c>
+      <c r="M8" s="8">
+        <v>5.6841943776152215</v>
+      </c>
+      <c r="N8" s="7">
+        <v>4.0976584515081971</v>
+      </c>
+      <c r="O8" s="8">
+        <v>10.902028376660384</v>
+      </c>
+      <c r="P8" s="8">
+        <v>1.8197530409203637</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>5.6841943776152215</v>
+      </c>
+      <c r="R8" s="7">
+        <v>0.25540271052969843</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0.55201633846561149</v>
+      </c>
+      <c r="T8" s="8">
+        <v>0.11326039556112689</v>
+      </c>
+      <c r="U8" s="8">
+        <v>0.32918675093335015</v>
+      </c>
       <c r="V8" s="7"/>
       <c r="W8" s="8"/>
       <c r="X8" s="6"/>
@@ -1267,6 +1316,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
@@ -1276,18 +1337,6 @@
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="R1:U1"/>
     <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1319,27 +1368,27 @@
         <v>5</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
       <c r="H1" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
@@ -1471,13 +1520,13 @@
         <v>3.6187068366596783E-4</v>
       </c>
       <c r="N3" s="14">
-        <v>7.1348626744966711E-7</v>
+        <v>2.1918969089406417E-7</v>
       </c>
       <c r="O3" s="15">
-        <v>1.0655828398642372E-4</v>
+        <v>1.4854612236429201E-6</v>
       </c>
       <c r="P3" s="15">
-        <v>3.6187068368761225E-4</v>
+        <v>3.6894005966918856E-6</v>
       </c>
       <c r="Q3" s="14"/>
       <c r="R3" s="15"/>
@@ -1530,13 +1579,13 @@
         <v>1.9630035394970443E-4</v>
       </c>
       <c r="N4" s="14">
-        <v>4.2926026937656802E-6</v>
+        <v>3.5098420073721417E-6</v>
       </c>
       <c r="O4" s="15">
-        <v>5.214686311404421E-5</v>
+        <v>1.3052042427009073E-5</v>
       </c>
       <c r="P4" s="15">
-        <v>1.9630035393360877E-4</v>
+        <v>2.3384914974048514E-5</v>
       </c>
       <c r="Q4" s="14"/>
       <c r="R4" s="15"/>
@@ -1589,13 +1638,13 @@
         <v>9.3813903988893878E-4</v>
       </c>
       <c r="N5" s="14">
-        <v>3.6570162465001113E-6</v>
+        <v>1.1021346262639836E-6</v>
       </c>
       <c r="O5" s="15">
-        <v>3.0200427863373802E-4</v>
+        <v>1.0731186519822165E-5</v>
       </c>
       <c r="P5" s="15">
-        <v>9.3813903988893878E-4</v>
+        <v>2.7035318413213515E-5</v>
       </c>
       <c r="Q5" s="14"/>
       <c r="R5" s="15"/>
@@ -1648,13 +1697,13 @@
         <v>6.2627529511751932E-4</v>
       </c>
       <c r="N6" s="14">
-        <v>1.6128209476273264E-5</v>
+        <v>1.2000447975481233E-5</v>
       </c>
       <c r="O6" s="15">
-        <v>1.5752489443211578E-4</v>
+        <v>6.483929182870517E-5</v>
       </c>
       <c r="P6" s="15">
-        <v>6.2077789815893089E-4</v>
+        <v>1.0680272134383506E-4</v>
       </c>
       <c r="Q6" s="14"/>
       <c r="R6" s="15"/>
@@ -1667,21 +1716,54 @@
       <c r="Y6" s="15"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1.0401824601280864E-5</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4.5616432177256166E-5</v>
+      </c>
+      <c r="D7" s="15">
+        <v>9.9321567102409215E-5</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1.0401824601280864E-5</v>
+      </c>
+      <c r="F7" s="15">
+        <v>4.5616432177256166E-5</v>
+      </c>
+      <c r="G7" s="15">
+        <v>9.9321567102409215E-5</v>
+      </c>
+      <c r="H7" s="14">
+        <v>1.7146171610124428E-5</v>
+      </c>
+      <c r="I7" s="15">
+        <v>1.6391900820663635E-4</v>
+      </c>
+      <c r="J7" s="15">
+        <v>7.0232332681102684E-4</v>
+      </c>
+      <c r="K7" s="14">
+        <v>1.7146171610124428E-5</v>
+      </c>
+      <c r="L7" s="15">
+        <v>1.6391900820663635E-4</v>
+      </c>
+      <c r="M7" s="15">
+        <v>7.0232332681102684E-4</v>
+      </c>
+      <c r="N7" s="14">
+        <v>7.4084404505763545E-8</v>
+      </c>
+      <c r="O7" s="15">
+        <v>1.4249529404123779E-6</v>
+      </c>
+      <c r="P7" s="15">
+        <v>3.3478383998289048E-6</v>
+      </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="15"/>
       <c r="S7" s="15"/>
@@ -1869,7 +1951,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1902,7 +1984,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="10">
         <v>5.1546980989150655E-3</v>
@@ -1922,7 +2004,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="10">
         <v>1.6135931931115562E-2</v>
@@ -1942,7 +2024,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="10">
         <v>7.092240261140333E-3</v>
@@ -1962,7 +2044,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="10">
         <v>1.8890501981792325E-2</v>
@@ -1982,7 +2064,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="10">
         <v>5.154698098915049E-3</v>
@@ -2002,7 +2084,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="10">
         <v>1.1563648163885921E-2</v>
@@ -2021,9 +2103,24 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="10"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2.4903862251546291E-3</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.286576149897383</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.12225740821148555</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>

</xml_diff>

<commit_message>
This is a checkpoint of a mostly sane state, after updating all the results tables from new runs.  But this update needs to be redone.
</commit_message>
<xml_diff>
--- a/calibration/overall_stats_cal_9_15_premo_cmu.xlsx
+++ b/calibration/overall_stats_cal_9_15_premo_cmu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_cal_data\cal_9_15_premo_cmu\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458C0CA2-4FBD-4D53-8055-83CC9FAB227B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63362E1A-683F-4157-B298-F86C98CC8B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="34560" windowHeight="19140" activeTab="2" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="24090" windowHeight="11775" activeTab="2" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Error stats" sheetId="1" r:id="rId1"/>
@@ -567,21 +567,21 @@
       <selection activeCell="R1" sqref="R1:U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="6" max="6" width="8.88671875" style="4"/>
-    <col min="10" max="10" width="8.88671875" style="4"/>
-    <col min="14" max="14" width="8.88671875" style="4"/>
-    <col min="18" max="18" width="8.88671875" style="4"/>
-    <col min="22" max="22" width="8.88671875" style="4"/>
-    <col min="25" max="25" width="8.88671875" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" style="4" customWidth="1"/>
-    <col min="30" max="30" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="4"/>
+    <col min="6" max="6" width="8.85546875" style="4"/>
+    <col min="10" max="10" width="8.85546875" style="4"/>
+    <col min="14" max="14" width="8.85546875" style="4"/>
+    <col min="18" max="18" width="8.85546875" style="4"/>
+    <col min="22" max="22" width="8.85546875" style="4"/>
+    <col min="25" max="25" width="8.85546875" customWidth="1"/>
+    <col min="26" max="26" width="8.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -624,7 +624,7 @@
       <c r="AB1" s="17"/>
       <c r="AC1" s="18"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="AC2" s="19"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,69 +771,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7">
-        <v>0.28068832614114686</v>
+        <v>0.26305582094218294</v>
       </c>
       <c r="C4" s="8">
-        <v>0.73440433276177086</v>
+        <v>0.72036761514221159</v>
       </c>
       <c r="D4" s="8">
-        <v>0.27469341877840853</v>
+        <v>0.27262142803520317</v>
       </c>
       <c r="E4" s="8">
-        <v>0.64227560401111072</v>
+        <v>0.63741010822327027</v>
       </c>
       <c r="F4" s="7">
-        <v>0.4334366747998819</v>
+        <v>0.4155529639662352</v>
       </c>
       <c r="G4" s="8">
-        <v>1.0968607376832644</v>
+        <v>1.0221359427840411</v>
       </c>
       <c r="H4" s="8">
-        <v>0.27469341877840853</v>
+        <v>0.27262142803520317</v>
       </c>
       <c r="I4" s="8">
-        <v>0.64227560401111072</v>
+        <v>0.63741010822327027</v>
       </c>
       <c r="J4" s="7">
-        <v>5.7193779810343397</v>
+        <v>5.6510629675715585</v>
       </c>
       <c r="K4" s="8">
-        <v>12.664857302939918</v>
+        <v>12.262207294192363</v>
       </c>
       <c r="L4" s="8">
-        <v>1.8246372218996534</v>
+        <v>1.826251405801596</v>
       </c>
       <c r="M4" s="8">
-        <v>5.2159749292658475</v>
+        <v>5.2217222544048152</v>
       </c>
       <c r="N4" s="7">
-        <v>4.5757703431194194</v>
+        <v>4.5804008317642193</v>
       </c>
       <c r="O4" s="8">
-        <v>12.402570780535587</v>
+        <v>12.255803737880138</v>
       </c>
       <c r="P4" s="8">
-        <v>1.8246372218996534</v>
+        <v>1.826251405801596</v>
       </c>
       <c r="Q4" s="8">
-        <v>5.2159749292658475</v>
+        <v>5.2217222544048152</v>
       </c>
       <c r="R4" s="7">
-        <v>0.44045419156778232</v>
+        <v>0.39591645281169513</v>
       </c>
       <c r="S4" s="8">
-        <v>1.0620358317544398</v>
+        <v>0.97679368462174154</v>
       </c>
       <c r="T4" s="8">
-        <v>0.26942241141433476</v>
+        <v>0.2758894906224868</v>
       </c>
       <c r="U4" s="8">
-        <v>0.48903093956696497</v>
+        <v>0.50137649258176764</v>
       </c>
       <c r="V4" s="7"/>
       <c r="W4" s="8"/>
@@ -844,69 +844,69 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="7">
-        <v>0.89609555096667726</v>
+        <v>0.89481118478916544</v>
       </c>
       <c r="C5" s="8">
-        <v>2.1941738410909193</v>
+        <v>2.2557770253709886</v>
       </c>
       <c r="D5" s="8">
-        <v>0.53910231829652577</v>
+        <v>0.5397699959736455</v>
       </c>
       <c r="E5" s="8">
-        <v>1.3845684193091312</v>
+        <v>1.3819778197344657</v>
       </c>
       <c r="F5" s="7">
-        <v>0.89609555096667726</v>
+        <v>0.89481118478916544</v>
       </c>
       <c r="G5" s="8">
-        <v>2.1941738410909193</v>
+        <v>2.2557770253709886</v>
       </c>
       <c r="H5" s="8">
-        <v>0.53910231829652577</v>
+        <v>0.5397699959736455</v>
       </c>
       <c r="I5" s="8">
-        <v>1.3845684193091312</v>
+        <v>1.3819778197344657</v>
       </c>
       <c r="J5" s="7">
-        <v>2.2963169785338899</v>
+        <v>2.3063463340270505</v>
       </c>
       <c r="K5" s="8">
-        <v>5.9709407594525068</v>
+        <v>6.1210123968581813</v>
       </c>
       <c r="L5" s="8">
-        <v>1.0974303795083338</v>
+        <v>1.099924631276439</v>
       </c>
       <c r="M5" s="8">
-        <v>3.400564659715593</v>
+        <v>3.3949064612528712</v>
       </c>
       <c r="N5" s="7">
-        <v>2.2963169785338899</v>
+        <v>2.3063463340270505</v>
       </c>
       <c r="O5" s="8">
-        <v>5.9709407594525068</v>
+        <v>6.1210123968581813</v>
       </c>
       <c r="P5" s="8">
-        <v>1.0974303795083338</v>
+        <v>1.099924631276439</v>
       </c>
       <c r="Q5" s="8">
-        <v>3.400564659715593</v>
+        <v>3.3949064612528712</v>
       </c>
       <c r="R5" s="7">
-        <v>0.86048770947841613</v>
+        <v>0.84429242751204736</v>
       </c>
       <c r="S5" s="8">
-        <v>1.746219106615871</v>
+        <v>1.7001852677224041</v>
       </c>
       <c r="T5" s="8">
-        <v>0.4013744777622526</v>
+        <v>0.39854538865688527</v>
       </c>
       <c r="U5" s="8">
-        <v>0.89751579883269172</v>
+        <v>0.88795241616779896</v>
       </c>
       <c r="V5" s="7"/>
       <c r="W5" s="8"/>
@@ -917,69 +917,69 @@
       <c r="AB5" s="8"/>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7">
-        <v>0.47338873693850109</v>
+        <v>0.46383884131970049</v>
       </c>
       <c r="C6" s="8">
-        <v>1.2639406414266798</v>
+        <v>1.2422811635137867</v>
       </c>
       <c r="D6" s="8">
-        <v>0.51090298228368991</v>
+        <v>0.50825270891314323</v>
       </c>
       <c r="E6" s="8">
-        <v>1.4147130140210986</v>
+        <v>1.4154726477601904</v>
       </c>
       <c r="F6" s="7">
-        <v>0.89970080651660578</v>
+        <v>0.90483646095157622</v>
       </c>
       <c r="G6" s="8">
-        <v>2.5883718045785824</v>
+        <v>2.4920522529965377</v>
       </c>
       <c r="H6" s="8">
-        <v>0.51090298228368991</v>
+        <v>0.50825270891314323</v>
       </c>
       <c r="I6" s="8">
-        <v>1.4147130140210986</v>
+        <v>1.4154726477601904</v>
       </c>
       <c r="J6" s="7">
-        <v>17.567171757536862</v>
+        <v>17.625301426948916</v>
       </c>
       <c r="K6" s="8">
-        <v>34.079012611828539</v>
+        <v>34.132884001940994</v>
       </c>
       <c r="L6" s="8">
-        <v>1.7777301511231276</v>
+        <v>1.7771684763249351</v>
       </c>
       <c r="M6" s="8">
-        <v>6.0029184201631915</v>
+        <v>5.9929813187270815</v>
       </c>
       <c r="N6" s="7">
-        <v>4.389302757355825</v>
+        <v>4.43539412592202</v>
       </c>
       <c r="O6" s="8">
-        <v>13.090889322656274</v>
+        <v>13.274209806295946</v>
       </c>
       <c r="P6" s="8">
-        <v>1.7777301511231276</v>
+        <v>1.7771684763249351</v>
       </c>
       <c r="Q6" s="8">
-        <v>6.0029184201631915</v>
+        <v>5.9929813187270815</v>
       </c>
       <c r="R6" s="7">
-        <v>0.77313860393405931</v>
+        <v>0.75371097655140729</v>
       </c>
       <c r="S6" s="8">
-        <v>1.911153534215704</v>
+        <v>1.8925775014526716</v>
       </c>
       <c r="T6" s="8">
-        <v>0.44334559757633096</v>
+        <v>0.44533942744904431</v>
       </c>
       <c r="U6" s="8">
-        <v>0.94597671130165861</v>
+        <v>0.94921387210318642</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" s="8"/>
@@ -990,69 +990,69 @@
       <c r="AB6" s="8"/>
       <c r="AC6" s="8"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="7">
-        <v>2.0960226951338661</v>
+        <v>2.1135867469472385</v>
       </c>
       <c r="C7" s="8">
-        <v>4.8527739510808656</v>
+        <v>4.9485215032370871</v>
       </c>
       <c r="D7" s="8">
-        <v>1.1048633974423512</v>
+        <v>1.1057872634239796</v>
       </c>
       <c r="E7" s="8">
-        <v>2.857977074784988</v>
+        <v>2.8551818025858986</v>
       </c>
       <c r="F7" s="7">
-        <v>2.0960226951338661</v>
+        <v>2.1135867469472385</v>
       </c>
       <c r="G7" s="8">
-        <v>4.8527739510808656</v>
+        <v>4.9485215032370871</v>
       </c>
       <c r="H7" s="8">
-        <v>1.1048633974423512</v>
+        <v>1.1057872634239796</v>
       </c>
       <c r="I7" s="8">
-        <v>2.857977074784988</v>
+        <v>2.8551818025858986</v>
       </c>
       <c r="J7" s="7">
-        <v>3.3593786984465095</v>
+        <v>3.385714487222474</v>
       </c>
       <c r="K7" s="8">
-        <v>9.1628312648326293</v>
+        <v>9.2198598422077485</v>
       </c>
       <c r="L7" s="8">
-        <v>1.6483812491916423</v>
+        <v>1.6500084838819615</v>
       </c>
       <c r="M7" s="8">
-        <v>4.9694351523684492</v>
+        <v>4.9642686890833003</v>
       </c>
       <c r="N7" s="7">
-        <v>3.3593786984465095</v>
+        <v>3.385714487222474</v>
       </c>
       <c r="O7" s="8">
-        <v>9.1628312648326293</v>
+        <v>9.2198598422077485</v>
       </c>
       <c r="P7" s="8">
-        <v>1.6483812491916423</v>
+        <v>1.6500084838819615</v>
       </c>
       <c r="Q7" s="8">
-        <v>4.9694351523684492</v>
+        <v>4.9642686890833003</v>
       </c>
       <c r="R7" s="7">
-        <v>1.8533410856640939</v>
+        <v>1.8611267033976833</v>
       </c>
       <c r="S7" s="8">
-        <v>3.8765000070625075</v>
+        <v>3.8695560586188642</v>
       </c>
       <c r="T7" s="8">
-        <v>0.969492110720096</v>
+        <v>0.96703056442154878</v>
       </c>
       <c r="U7" s="8">
-        <v>2.0090363659847279</v>
+        <v>2.0063902649881955</v>
       </c>
       <c r="V7" s="7"/>
       <c r="W7" s="8"/>
@@ -1063,76 +1063,76 @@
       <c r="AB7" s="8"/>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="7">
-        <v>2.0161262455969489</v>
+        <v>1.8522739870382945</v>
       </c>
       <c r="C8" s="8">
-        <v>6.0723151510827398</v>
+        <v>5.4077548902666175</v>
       </c>
       <c r="D8" s="8">
-        <v>1.1608734504931362</v>
+        <v>1.0877705935526274</v>
       </c>
       <c r="E8" s="8">
-        <v>3.0251112642908211</v>
+        <v>2.8094892492260954</v>
       </c>
       <c r="F8" s="7">
-        <v>2.0195603550988559</v>
+        <v>1.8622583486217901</v>
       </c>
       <c r="G8" s="8">
-        <v>6.2161674725761831</v>
+        <v>5.5141254897433791</v>
       </c>
       <c r="H8" s="8">
-        <v>1.1608734504931362</v>
+        <v>1.0877705935526274</v>
       </c>
       <c r="I8" s="8">
-        <v>3.0251112642908211</v>
+        <v>2.8094892492260954</v>
       </c>
       <c r="J8" s="7">
-        <v>4.0425154984316869</v>
+        <v>4.0452096467030438</v>
       </c>
       <c r="K8" s="8">
-        <v>10.319847881624611</v>
+        <v>10.671151071301688</v>
       </c>
       <c r="L8" s="8">
-        <v>1.8197530409203637</v>
+        <v>1.7929585546385536</v>
       </c>
       <c r="M8" s="8">
-        <v>5.6841943776152215</v>
+        <v>5.6715502299317091</v>
       </c>
       <c r="N8" s="7">
-        <v>4.0976584515081971</v>
+        <v>4.1217087686598237</v>
       </c>
       <c r="O8" s="8">
-        <v>10.902028376660384</v>
+        <v>11.226910693298466</v>
       </c>
       <c r="P8" s="8">
-        <v>1.8197530409203637</v>
+        <v>1.7929585546385536</v>
       </c>
       <c r="Q8" s="8">
-        <v>5.6841943776152215</v>
+        <v>5.6715502299317091</v>
       </c>
       <c r="R8" s="7">
-        <v>0.25540271052969843</v>
+        <v>0.23082321068508216</v>
       </c>
       <c r="S8" s="8">
-        <v>0.55201633846561149</v>
+        <v>0.61278474561095564</v>
       </c>
       <c r="T8" s="8">
-        <v>0.11326039556112689</v>
+        <v>0.10886736530310946</v>
       </c>
       <c r="U8" s="8">
-        <v>0.32918675093335015</v>
+        <v>0.30773206977692641</v>
       </c>
       <c r="V8" s="7"/>
       <c r="W8" s="8"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1158,7 +1158,7 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1184,7 +1184,7 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1210,7 +1210,7 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1236,7 +1236,7 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1262,7 +1262,7 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1288,7 +1288,7 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1350,20 +1350,20 @@
       <selection activeCell="N1" sqref="N1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="5" max="5" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="8.88671875" style="4"/>
-    <col min="11" max="11" width="8.88671875" style="4"/>
-    <col min="14" max="14" width="8.88671875" style="4"/>
-    <col min="17" max="17" width="8.88671875" style="4"/>
-    <col min="20" max="20" width="8.88671875" style="4"/>
-    <col min="23" max="23" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="4"/>
+    <col min="5" max="5" width="8.85546875" style="4"/>
+    <col min="8" max="8" width="8.85546875" style="4"/>
+    <col min="11" max="11" width="8.85546875" style="4"/>
+    <col min="14" max="14" width="8.85546875" style="4"/>
+    <col min="17" max="17" width="8.85546875" style="4"/>
+    <col min="20" max="20" width="8.85546875" style="4"/>
+    <col min="23" max="23" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="X1" s="17"/>
       <c r="Y1" s="17"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1479,54 +1479,54 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="14">
-        <v>2.429088881590778E-7</v>
+        <v>2.438730695208001E-7</v>
       </c>
       <c r="C3" s="15">
-        <v>1.7072629205736015E-6</v>
+        <v>1.6820038199546791E-6</v>
       </c>
       <c r="D3" s="15">
-        <v>6.1548215137103984E-6</v>
+        <v>5.636760207921096E-6</v>
       </c>
       <c r="E3" s="14">
-        <v>2.429088881590778E-7</v>
+        <v>2.438730695208001E-7</v>
       </c>
       <c r="F3" s="15">
-        <v>1.7072629205736015E-6</v>
+        <v>1.6820038199546791E-6</v>
       </c>
       <c r="G3" s="15">
-        <v>6.1548215137103984E-6</v>
+        <v>5.636760207921096E-6</v>
       </c>
       <c r="H3" s="14">
-        <v>1.8889013780695625E-6</v>
+        <v>1.9177930179513455E-6</v>
       </c>
       <c r="I3" s="15">
-        <v>1.2513914800043439E-4</v>
+        <v>1.2454535336829857E-4</v>
       </c>
       <c r="J3" s="15">
-        <v>3.6187068366596783E-4</v>
+        <v>3.7107016434581201E-4</v>
       </c>
       <c r="K3" s="14">
-        <v>1.8889013780695625E-6</v>
+        <v>1.9177930179513455E-6</v>
       </c>
       <c r="L3" s="15">
-        <v>1.2513914800043439E-4</v>
+        <v>1.2454535336829857E-4</v>
       </c>
       <c r="M3" s="15">
-        <v>3.6187068366596783E-4</v>
+        <v>3.7107016434581201E-4</v>
       </c>
       <c r="N3" s="14">
-        <v>2.1918969089406417E-7</v>
+        <v>2.2704237737513087E-7</v>
       </c>
       <c r="O3" s="15">
-        <v>1.4854612236429201E-6</v>
+        <v>1.6212101582340842E-6</v>
       </c>
       <c r="P3" s="15">
-        <v>3.6894005966918856E-6</v>
+        <v>3.1299102398856622E-6</v>
       </c>
       <c r="Q3" s="14"/>
       <c r="R3" s="15"/>
@@ -1538,54 +1538,54 @@
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="14">
-        <v>3.2441355523633714E-6</v>
+        <v>3.2259314692600019E-6</v>
       </c>
       <c r="C4" s="15">
-        <v>1.2805817331408957E-5</v>
+        <v>1.271889189521714E-5</v>
       </c>
       <c r="D4" s="15">
-        <v>2.6481099218255339E-5</v>
+        <v>2.7270402977647394E-5</v>
       </c>
       <c r="E4" s="14">
-        <v>3.2441355523633714E-6</v>
+        <v>3.2259314692600019E-6</v>
       </c>
       <c r="F4" s="15">
-        <v>1.2805817331408957E-5</v>
+        <v>1.271889189521714E-5</v>
       </c>
       <c r="G4" s="15">
-        <v>2.6481099218255339E-5</v>
+        <v>2.7270402977647394E-5</v>
       </c>
       <c r="H4" s="14">
-        <v>5.4168415598420516E-6</v>
+        <v>5.4053204388984008E-6</v>
       </c>
       <c r="I4" s="15">
-        <v>5.449314191254583E-5</v>
+        <v>5.4586689222366261E-5</v>
       </c>
       <c r="J4" s="15">
-        <v>1.9630035394970443E-4</v>
+        <v>1.951213656466319E-4</v>
       </c>
       <c r="K4" s="14">
-        <v>5.4168415598420516E-6</v>
+        <v>5.4053204388984008E-6</v>
       </c>
       <c r="L4" s="15">
-        <v>5.449314191254583E-5</v>
+        <v>5.4586689222366261E-5</v>
       </c>
       <c r="M4" s="15">
-        <v>1.9630035394970443E-4</v>
+        <v>1.951213656466319E-4</v>
       </c>
       <c r="N4" s="14">
-        <v>3.5098420073721417E-6</v>
+        <v>3.5923260842485733E-6</v>
       </c>
       <c r="O4" s="15">
-        <v>1.3052042427009073E-5</v>
+        <v>1.3469055147008322E-5</v>
       </c>
       <c r="P4" s="15">
-        <v>2.3384914974048514E-5</v>
+        <v>2.4146027201324982E-5</v>
       </c>
       <c r="Q4" s="14"/>
       <c r="R4" s="15"/>
@@ -1597,54 +1597,54 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="15"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="14">
-        <v>1.2331809450701004E-6</v>
+        <v>1.263394099378745E-6</v>
       </c>
       <c r="C5" s="15">
-        <v>1.0290382737264169E-5</v>
+        <v>1.0100891702989706E-5</v>
       </c>
       <c r="D5" s="15">
-        <v>3.091496142669584E-5</v>
+        <v>3.0356332422134922E-5</v>
       </c>
       <c r="E5" s="14">
-        <v>1.2331809450701004E-6</v>
+        <v>1.263394099378745E-6</v>
       </c>
       <c r="F5" s="15">
-        <v>1.0290382737264169E-5</v>
+        <v>1.0100891702989706E-5</v>
       </c>
       <c r="G5" s="15">
-        <v>3.091496142669584E-5</v>
+        <v>3.0356332422134922E-5</v>
       </c>
       <c r="H5" s="14">
-        <v>2.3001194593479631E-5</v>
+        <v>2.3055611004972053E-5</v>
       </c>
       <c r="I5" s="15">
-        <v>3.8043981308869928E-4</v>
+        <v>3.8132519198662621E-4</v>
       </c>
       <c r="J5" s="15">
-        <v>9.3813903988893878E-4</v>
+        <v>9.3841936080942532E-4</v>
       </c>
       <c r="K5" s="14">
-        <v>2.3001194593479631E-5</v>
+        <v>2.3055611004972053E-5</v>
       </c>
       <c r="L5" s="15">
-        <v>3.8043981308869928E-4</v>
+        <v>3.8132519198662621E-4</v>
       </c>
       <c r="M5" s="15">
-        <v>9.3813903988893878E-4</v>
+        <v>9.3841936080942532E-4</v>
       </c>
       <c r="N5" s="14">
-        <v>1.1021346262639836E-6</v>
+        <v>1.1270424438709884E-6</v>
       </c>
       <c r="O5" s="15">
-        <v>1.0731186519822165E-5</v>
+        <v>1.042246146403191E-5</v>
       </c>
       <c r="P5" s="15">
-        <v>2.7035318413213515E-5</v>
+        <v>2.6448157741827448E-5</v>
       </c>
       <c r="Q5" s="14"/>
       <c r="R5" s="15"/>
@@ -1656,54 +1656,54 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="15"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="14">
-        <v>1.2205502848652424E-5</v>
+        <v>1.212947106223915E-5</v>
       </c>
       <c r="C6" s="15">
-        <v>7.2994631523980313E-5</v>
+        <v>7.2134540235145367E-5</v>
       </c>
       <c r="D6" s="15">
-        <v>1.8453154857864075E-4</v>
+        <v>1.8487084031614684E-4</v>
       </c>
       <c r="E6" s="14">
-        <v>1.2205502848652424E-5</v>
+        <v>1.212947106223915E-5</v>
       </c>
       <c r="F6" s="15">
-        <v>7.2994631523980313E-5</v>
+        <v>7.2134540235145367E-5</v>
       </c>
       <c r="G6" s="15">
-        <v>1.8453154857864075E-4</v>
+        <v>1.8487084031614684E-4</v>
       </c>
       <c r="H6" s="14">
-        <v>2.3268298141223465E-5</v>
+        <v>2.3209578308370339E-5</v>
       </c>
       <c r="I6" s="15">
-        <v>2.276818943510682E-4</v>
+        <v>2.2733395891573065E-4</v>
       </c>
       <c r="J6" s="15">
-        <v>6.2627529511751932E-4</v>
+        <v>6.2722240652542669E-4</v>
       </c>
       <c r="K6" s="14">
-        <v>2.3268298141223465E-5</v>
+        <v>2.3209578308370339E-5</v>
       </c>
       <c r="L6" s="15">
-        <v>2.276818943510682E-4</v>
+        <v>2.2733395891573065E-4</v>
       </c>
       <c r="M6" s="15">
-        <v>6.2627529511751932E-4</v>
+        <v>6.2722240652542669E-4</v>
       </c>
       <c r="N6" s="14">
-        <v>1.2000447975481233E-5</v>
+        <v>1.2012172335041604E-5</v>
       </c>
       <c r="O6" s="15">
-        <v>6.483929182870517E-5</v>
+        <v>6.4639030154078916E-5</v>
       </c>
       <c r="P6" s="15">
-        <v>1.0680272134383506E-4</v>
+        <v>1.0635465834533318E-4</v>
       </c>
       <c r="Q6" s="14"/>
       <c r="R6" s="15"/>
@@ -1715,54 +1715,54 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="15"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="14">
-        <v>1.0401824601280864E-5</v>
+        <v>8.6720698499263082E-6</v>
       </c>
       <c r="C7" s="15">
-        <v>4.5616432177256166E-5</v>
+        <v>3.7701660112795592E-5</v>
       </c>
       <c r="D7" s="15">
-        <v>9.9321567102409215E-5</v>
+        <v>7.9777910310080196E-5</v>
       </c>
       <c r="E7" s="14">
-        <v>1.0401824601280864E-5</v>
+        <v>8.6720698499263082E-6</v>
       </c>
       <c r="F7" s="15">
-        <v>4.5616432177256166E-5</v>
+        <v>3.7701660112795592E-5</v>
       </c>
       <c r="G7" s="15">
-        <v>9.9321567102409215E-5</v>
+        <v>7.9777910310080196E-5</v>
       </c>
       <c r="H7" s="14">
-        <v>1.7146171610124428E-5</v>
+        <v>1.5265253410505826E-5</v>
       </c>
       <c r="I7" s="15">
-        <v>1.6391900820663635E-4</v>
+        <v>1.5826100014507049E-4</v>
       </c>
       <c r="J7" s="15">
-        <v>7.0232332681102684E-4</v>
+        <v>6.7237737738070388E-4</v>
       </c>
       <c r="K7" s="14">
-        <v>1.7146171610124428E-5</v>
+        <v>1.5265253410505826E-5</v>
       </c>
       <c r="L7" s="15">
-        <v>1.6391900820663635E-4</v>
+        <v>1.5826100014507049E-4</v>
       </c>
       <c r="M7" s="15">
-        <v>7.0232332681102684E-4</v>
+        <v>6.7237737738070388E-4</v>
       </c>
       <c r="N7" s="14">
-        <v>7.4084404505763545E-8</v>
+        <v>8.0254631853129557E-8</v>
       </c>
       <c r="O7" s="15">
-        <v>1.4249529404123779E-6</v>
+        <v>1.2226028866690741E-6</v>
       </c>
       <c r="P7" s="15">
-        <v>3.3478383998289048E-6</v>
+        <v>2.6019493856997296E-6</v>
       </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="15"/>
@@ -1774,7 +1774,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="15"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -1800,7 +1800,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="15"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -1826,7 +1826,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="15"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -1852,7 +1852,7 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1878,7 +1878,7 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1904,7 +1904,7 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1954,15 +1954,15 @@
       <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="4" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1982,12 +1982,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="10">
-        <v>5.1546980989150655E-3</v>
+        <v>4.8470969926311591E-3</v>
       </c>
       <c r="C2">
         <v>426</v>
@@ -2002,12 +2002,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="10">
-        <v>1.6135931931115562E-2</v>
+        <v>1.6104433207496681E-2</v>
       </c>
       <c r="C3">
         <v>852</v>
@@ -2022,12 +2022,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="10">
-        <v>7.092240261140333E-3</v>
+        <v>6.9491527085798668E-3</v>
       </c>
       <c r="C4">
         <v>426</v>
@@ -2036,24 +2036,24 @@
         <v>21</v>
       </c>
       <c r="E4" s="8">
-        <v>1.0145559006065887</v>
+        <v>1.0393727343991754</v>
       </c>
       <c r="F4" s="8">
-        <v>0.45372504510886946</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.45059431880421669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="10">
-        <v>1.8890501981792325E-2</v>
+        <v>1.8888655887120288E-2</v>
       </c>
       <c r="C5">
         <v>852</v>
       </c>
       <c r="D5">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E5" s="8">
         <v>0</v>
@@ -2062,12 +2062,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="10">
-        <v>5.154698098915049E-3</v>
+        <v>4.8470969926290314E-3</v>
       </c>
       <c r="C6">
         <v>426</v>
@@ -2076,24 +2076,24 @@
         <v>0</v>
       </c>
       <c r="E6" s="8">
-        <v>0.515294609241572</v>
+        <v>0.46909255883060097</v>
       </c>
       <c r="F6" s="8">
-        <v>0.30090708326537929</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.27760645779304266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="10">
-        <v>1.1563648163885921E-2</v>
+        <v>1.1496509946386685E-2</v>
       </c>
       <c r="C7">
         <v>852</v>
       </c>
       <c r="D7">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
@@ -2102,12 +2102,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="10">
-        <v>2.4903862251546291E-3</v>
+        <v>1.8344973934603689E-3</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -2116,69 +2116,69 @@
         <v>0</v>
       </c>
       <c r="E8" s="8">
-        <v>0.286576149897383</v>
+        <v>0.26005477768738072</v>
       </c>
       <c r="F8" s="8">
-        <v>0.12225740821148555</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.11807142260126582</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="9"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated all the data tables and linearity plots, added new photo of the fixture positions. Reworked the stage discussion a bit.
</commit_message>
<xml_diff>
--- a/calibration/overall_stats_cal_9_15_premo_cmu.xlsx
+++ b/calibration/overall_stats_cal_9_15_premo_cmu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_cal_data\cal_9_15_premo_cmu\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63362E1A-683F-4157-B298-F86C98CC8B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5281EDD-DD31-406A-83EA-A5FAAE79606E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="24090" windowHeight="11775" activeTab="2" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
+    <workbookView xWindow="2712" yWindow="2712" windowWidth="20352" windowHeight="10272" activeTab="2" xr2:uid="{5D7C67CD-972B-4CBF-BC15-D765573F58E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Error stats" sheetId="1" r:id="rId1"/>
@@ -567,21 +567,21 @@
       <selection activeCell="R1" sqref="R1:U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="4"/>
-    <col min="6" max="6" width="8.85546875" style="4"/>
-    <col min="10" max="10" width="8.85546875" style="4"/>
-    <col min="14" max="14" width="8.85546875" style="4"/>
-    <col min="18" max="18" width="8.85546875" style="4"/>
-    <col min="22" max="22" width="8.85546875" style="4"/>
-    <col min="25" max="25" width="8.85546875" customWidth="1"/>
-    <col min="26" max="26" width="8.85546875" style="4" customWidth="1"/>
-    <col min="30" max="30" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="10" max="10" width="8.88671875" style="4"/>
+    <col min="14" max="14" width="8.88671875" style="4"/>
+    <col min="18" max="18" width="8.88671875" style="4"/>
+    <col min="22" max="22" width="8.88671875" style="4"/>
+    <col min="25" max="25" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="8.88671875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -624,7 +624,7 @@
       <c r="AB1" s="17"/>
       <c r="AC1" s="18"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
@@ -682,7 +682,7 @@
       </c>
       <c r="AC2" s="19"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,7 +771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -844,7 +844,7 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -917,7 +917,7 @@
       <c r="AB5" s="8"/>
       <c r="AC5" s="8"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="AB6" s="8"/>
       <c r="AC6" s="8"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1063,7 +1063,7 @@
       <c r="AB7" s="8"/>
       <c r="AC7" s="8"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1158,7 +1158,7 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1184,7 +1184,7 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -1210,7 +1210,7 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1236,7 +1236,7 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1262,7 +1262,7 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1288,7 +1288,7 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1350,20 +1350,20 @@
       <selection activeCell="N1" sqref="N1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="4"/>
-    <col min="5" max="5" width="8.85546875" style="4"/>
-    <col min="8" max="8" width="8.85546875" style="4"/>
-    <col min="11" max="11" width="8.85546875" style="4"/>
-    <col min="14" max="14" width="8.85546875" style="4"/>
-    <col min="17" max="17" width="8.85546875" style="4"/>
-    <col min="20" max="20" width="8.85546875" style="4"/>
-    <col min="23" max="23" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
+    <col min="11" max="11" width="8.88671875" style="4"/>
+    <col min="14" max="14" width="8.88671875" style="4"/>
+    <col min="17" max="17" width="8.88671875" style="4"/>
+    <col min="20" max="20" width="8.88671875" style="4"/>
+    <col min="23" max="23" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="X1" s="17"/>
       <c r="Y1" s="17"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1538,7 +1538,7 @@
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1597,7 +1597,7 @@
       <c r="X4" s="15"/>
       <c r="Y4" s="15"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="X5" s="15"/>
       <c r="Y5" s="15"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="X6" s="15"/>
       <c r="Y6" s="15"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="X7" s="15"/>
       <c r="Y7" s="15"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -1800,7 +1800,7 @@
       <c r="X8" s="15"/>
       <c r="Y8" s="15"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -1826,7 +1826,7 @@
       <c r="X9" s="15"/>
       <c r="Y9" s="15"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -1852,7 +1852,7 @@
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1878,7 +1878,7 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1904,7 +1904,7 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1954,15 +1954,15 @@
       <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>0.45059431880421669</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>0.27760645779304266</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2122,63 +2122,63 @@
         <v>0.11807142260126582</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="9"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="9"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="9"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="9"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="9"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" s="9"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="9"/>
     </row>
   </sheetData>

</xml_diff>